<commit_message>
i honestly dont know how to name these fixes anymore
</commit_message>
<xml_diff>
--- a/LR3/table_1_78.xlsx
+++ b/LR3/table_1_78.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{484CA18C-E266-4892-866C-9FF252C45C90}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3B2AD9-47B6-4E43-8C57-F1324B61B9EC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2003,12 +2003,12 @@
         <v>54</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="7"/>
-        <v>85.800000000000011</v>
+        <f>$D$3/2</f>
+        <v>42.900000000000006</v>
       </c>
       <c r="E35" s="5">
         <f t="shared" si="0"/>
-        <v>4633.2000000000007</v>
+        <v>2316.6000000000004</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="K35" s="7">
         <f t="shared" si="4"/>
-        <v>4873.2000000000007</v>
+        <v>2556.6000000000004</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2047,12 +2047,12 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="7"/>
-        <v>85.800000000000011</v>
+        <f t="shared" ref="D36:D38" si="9">$D$3/2</f>
+        <v>42.900000000000006</v>
       </c>
       <c r="E36" s="5">
         <f t="shared" si="0"/>
-        <v>4590.3</v>
+        <v>2295.15</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="1"/>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="K36" s="7">
         <f t="shared" si="4"/>
-        <v>4840.3</v>
+        <v>2545.15</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2091,7 +2091,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="1">
-        <f>D3/2</f>
+        <f t="shared" si="9"/>
         <v>42.900000000000006</v>
       </c>
       <c r="E37" s="5">
@@ -2135,7 +2135,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="1">
-        <f>D4/2</f>
+        <f t="shared" si="9"/>
         <v>42.900000000000006</v>
       </c>
       <c r="E38" s="5">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="C40" s="7">
         <f>FLOOR(SUM(K3:K38),1)</f>
-        <v>188443</v>
+        <v>183831</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ok it should work now
</commit_message>
<xml_diff>
--- a/LR3/table_1_78.xlsx
+++ b/LR3/table_1_78.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3B2AD9-47B6-4E43-8C57-F1324B61B9EC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAA9B61-353B-4FB7-AF8F-66C2D05A5662}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -683,7 +683,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D36" si="7">D4</f>
+        <f t="shared" ref="D5:D34" si="7">D4</f>
         <v>85.800000000000011</v>
       </c>
       <c r="E5" s="5">
@@ -2003,12 +2003,12 @@
         <v>54</v>
       </c>
       <c r="D35" s="1">
-        <f>$D$3/2</f>
-        <v>42.900000000000006</v>
+        <f>$D$3/3</f>
+        <v>28.600000000000005</v>
       </c>
       <c r="E35" s="5">
         <f t="shared" si="0"/>
-        <v>2316.6000000000004</v>
+        <v>1544.4000000000003</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="K35" s="7">
         <f t="shared" si="4"/>
-        <v>2556.6000000000004</v>
+        <v>1784.4000000000003</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2047,12 +2047,12 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" ref="D36:D38" si="9">$D$3/2</f>
-        <v>42.900000000000006</v>
+        <f t="shared" ref="D36:D38" si="9">$D$3/3</f>
+        <v>28.600000000000005</v>
       </c>
       <c r="E36" s="5">
         <f t="shared" si="0"/>
-        <v>2295.15</v>
+        <v>1530.1000000000004</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="1"/>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="K36" s="7">
         <f t="shared" si="4"/>
-        <v>2545.15</v>
+        <v>1780.1000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2092,11 +2092,11 @@
       </c>
       <c r="D37" s="1">
         <f t="shared" si="9"/>
-        <v>42.900000000000006</v>
+        <v>28.600000000000005</v>
       </c>
       <c r="E37" s="5">
         <f t="shared" si="0"/>
-        <v>2273.7000000000003</v>
+        <v>1515.8000000000002</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="1"/>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="K37" s="7">
         <f t="shared" si="4"/>
-        <v>2533.7000000000003</v>
+        <v>1775.8000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2136,11 +2136,11 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" si="9"/>
-        <v>42.900000000000006</v>
+        <v>28.600000000000005</v>
       </c>
       <c r="E38" s="5">
         <f t="shared" si="0"/>
-        <v>2252.2500000000005</v>
+        <v>1501.5000000000002</v>
       </c>
       <c r="F38" s="3">
         <f t="shared" si="1"/>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="K38" s="7">
         <f t="shared" si="4"/>
-        <v>2522.2500000000005</v>
+        <v>1771.5000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="C40" s="7">
         <f>FLOOR(SUM(K3:K38),1)</f>
-        <v>183831</v>
+        <v>180785</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
progress is being made
</commit_message>
<xml_diff>
--- a/LR3/table_1_78.xlsx
+++ b/LR3/table_1_78.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAA9B61-353B-4FB7-AF8F-66C2D05A5662}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB43CE0-A1FD-4451-B7F8-A4339C4BB9D6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2003,12 +2003,12 @@
         <v>54</v>
       </c>
       <c r="D35" s="1">
-        <f>$D$3/3</f>
-        <v>28.600000000000005</v>
+        <f>D3/2</f>
+        <v>42.900000000000006</v>
       </c>
       <c r="E35" s="5">
         <f t="shared" si="0"/>
-        <v>1544.4000000000003</v>
+        <v>2316.6000000000004</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="K35" s="7">
         <f t="shared" si="4"/>
-        <v>1784.4000000000003</v>
+        <v>2556.6000000000004</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2047,12 +2047,12 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" ref="D36:D38" si="9">$D$3/3</f>
-        <v>28.600000000000005</v>
+        <f>D3/2</f>
+        <v>42.900000000000006</v>
       </c>
       <c r="E36" s="5">
         <f t="shared" si="0"/>
-        <v>1530.1000000000004</v>
+        <v>2295.15</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="1"/>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="K36" s="7">
         <f t="shared" si="4"/>
-        <v>1780.1000000000004</v>
+        <v>2545.15</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2091,12 +2091,12 @@
         <v>53</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="9"/>
-        <v>28.600000000000005</v>
+        <f>D3/2</f>
+        <v>42.900000000000006</v>
       </c>
       <c r="E37" s="5">
         <f t="shared" si="0"/>
-        <v>1515.8000000000002</v>
+        <v>2273.7000000000003</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="1"/>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="K37" s="7">
         <f t="shared" si="4"/>
-        <v>1775.8000000000002</v>
+        <v>2533.7000000000003</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2135,12 +2135,12 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="9"/>
-        <v>28.600000000000005</v>
+        <f>D3/2</f>
+        <v>42.900000000000006</v>
       </c>
       <c r="E38" s="5">
         <f t="shared" si="0"/>
-        <v>1501.5000000000002</v>
+        <v>2252.2500000000005</v>
       </c>
       <c r="F38" s="3">
         <f t="shared" si="1"/>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="K38" s="7">
         <f t="shared" si="4"/>
-        <v>1771.5000000000002</v>
+        <v>2522.2500000000005</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="C40" s="7">
         <f>FLOOR(SUM(K3:K38),1)</f>
-        <v>180785</v>
+        <v>183831</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
i dont know whats wrong with this one tbh
</commit_message>
<xml_diff>
--- a/LR3/table_1_78.xlsx
+++ b/LR3/table_1_78.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC33E2AA-D3B2-48E3-B446-3318085762C4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BEE397-3F3F-4144-B001-196408FA2A3A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2003,12 +2003,12 @@
         <v>54</v>
       </c>
       <c r="D35" s="1">
-        <f>D3/3</f>
-        <v>28.600000000000005</v>
+        <f>($A$1*1.1)/2</f>
+        <v>42.900000000000006</v>
       </c>
       <c r="E35" s="5">
         <f t="shared" si="0"/>
-        <v>1544.4000000000003</v>
+        <v>2316.6000000000004</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="K35" s="7">
         <f t="shared" si="4"/>
-        <v>1784.4000000000003</v>
+        <v>2556.6000000000004</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2047,12 +2047,12 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
-        <f>D3/3</f>
-        <v>28.600000000000005</v>
+        <f t="shared" ref="D36:D38" si="9">($A$1*1.1)/2</f>
+        <v>42.900000000000006</v>
       </c>
       <c r="E36" s="5">
         <f t="shared" si="0"/>
-        <v>1530.1000000000004</v>
+        <v>2295.15</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="1"/>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="K36" s="7">
         <f t="shared" si="4"/>
-        <v>1780.1000000000004</v>
+        <v>2545.15</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2091,12 +2091,12 @@
         <v>53</v>
       </c>
       <c r="D37" s="1">
-        <f>D3/3</f>
-        <v>28.600000000000005</v>
+        <f t="shared" si="9"/>
+        <v>42.900000000000006</v>
       </c>
       <c r="E37" s="5">
         <f t="shared" si="0"/>
-        <v>1515.8000000000002</v>
+        <v>2273.7000000000003</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="1"/>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="K37" s="7">
         <f t="shared" si="4"/>
-        <v>1775.8000000000002</v>
+        <v>2533.7000000000003</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2135,12 +2135,12 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="1">
-        <f>D3/3</f>
-        <v>28.600000000000005</v>
+        <f t="shared" si="9"/>
+        <v>42.900000000000006</v>
       </c>
       <c r="E38" s="5">
         <f t="shared" si="0"/>
-        <v>1501.5000000000002</v>
+        <v>2252.2500000000005</v>
       </c>
       <c r="F38" s="3">
         <f t="shared" si="1"/>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="K38" s="7">
         <f t="shared" si="4"/>
-        <v>1771.5000000000002</v>
+        <v>2522.2500000000005</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="C40" s="7">
         <f>FLOOR(SUM(K3:K38),1)</f>
-        <v>180785</v>
+        <v>183831</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
i dont know whats wrong
</commit_message>
<xml_diff>
--- a/LR3/table_1_78.xlsx
+++ b/LR3/table_1_78.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BEE397-3F3F-4144-B001-196408FA2A3A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E905B59-F964-4477-949B-87359F219BBC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35:D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2003,7 +2003,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="1">
-        <f>($A$1*1.1)/2</f>
+        <f>$D$3/2</f>
         <v>42.900000000000006</v>
       </c>
       <c r="E35" s="5">
@@ -2047,7 +2047,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" ref="D36:D38" si="9">($A$1*1.1)/2</f>
+        <f t="shared" ref="D36:D38" si="9">$D$3/2</f>
         <v>42.900000000000006</v>
       </c>
       <c r="E36" s="5">

</xml_diff>